<commit_message>
Perbaiki beberapa kondisi pada impr data vaksin
</commit_message>
<xml_diff>
--- a/assets/import/FormatImporVaksin.xlsx
+++ b/assets/import/FormatImporVaksin.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenDesa\OpenSID\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6DCA77-BBED-4062-B699-603D7B93BDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9010E29-2ADC-4ABE-AEDE-0BF285630832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="208" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vaksin" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Referensi" sheetId="3" r:id="rId2"/>
+    <sheet name="Catatan" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>NIK</t>
   </si>
@@ -35,12 +35,6 @@
     <t>JENIS VAKSIN 1</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2022-02-17</t>
-  </si>
-  <si>
     <t>AstraZeneca</t>
   </si>
   <si>
@@ -50,12 +44,6 @@
     <t>Sinovac</t>
   </si>
   <si>
-    <t>2022-02-18</t>
-  </si>
-  <si>
-    <t>2022-02-19</t>
-  </si>
-  <si>
     <t>TANGGAL VAKSIN 2</t>
   </si>
   <si>
@@ -68,39 +56,12 @@
     <t>JENIS VAKSIN 3</t>
   </si>
   <si>
-    <t>2022-03-20</t>
-  </si>
-  <si>
-    <t>2022-03-23</t>
-  </si>
-  <si>
-    <t>TUNDA</t>
-  </si>
-  <si>
     <t>KETERANGAN</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Tekanan darah tinggi</t>
-  </si>
-  <si>
-    <t>5201143112707040</t>
-  </si>
-  <si>
-    <t>5201143105121724</t>
-  </si>
-  <si>
-    <t>5201145107836994</t>
-  </si>
-  <si>
     <t>5201143112897123</t>
   </si>
   <si>
-    <t>Jenis Vaksin</t>
-  </si>
-  <si>
     <t>Covovax</t>
   </si>
   <si>
@@ -122,13 +83,70 @@
     <t>Biofarma</t>
   </si>
   <si>
-    <t>Tunda</t>
-  </si>
-  <si>
-    <t>Tidak</t>
-  </si>
-  <si>
-    <t>Ya</t>
+    <t>2022-01-01</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Kolom Isian</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1. Terdaftar pada data penduduk dan masih hidup</t>
+  </si>
+  <si>
+    <t>Referensi</t>
+  </si>
+  <si>
+    <t>2. Isi berdasarkan data referensi</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>2021-12-01</t>
+  </si>
+  <si>
+    <t>2022-02-01</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Lainnya</t>
+  </si>
+  <si>
+    <t>1. Jika diisi, status vaksin dinyatakan tunda</t>
+  </si>
+  <si>
+    <t>3. Lainnya, data tidak tersimpan</t>
+  </si>
+  <si>
+    <t>1. Format tgl adalah yyyy-mm-dd (mis: 2022-02-22)</t>
+  </si>
+  <si>
+    <t>Tanggal Vaksin [1, 2, 3]</t>
+  </si>
+  <si>
+    <t>Jenis Vaksin [1, 2, 3]</t>
+  </si>
+  <si>
+    <t>2. Jika format tgl tidak valid, data vaksin [1, 2, 3] tsb tidak tersimpan</t>
+  </si>
+  <si>
+    <t>1. Isi manual (bebas asal tidak kosong) selain dari data referensi</t>
+  </si>
+  <si>
+    <t>1. Data vaksin 1, 2, 3 disimpan secara berurutan (tidak boleh lompat)</t>
+  </si>
+  <si>
+    <t>2. Jika tdk diisi dan tgl vaksin 1 harus valid</t>
+  </si>
+  <si>
+    <t>3. Jika kosong akan diisi default (Covovax) untuk vaksin 1, sendangkan vaksin 2 atau 3 disi sesuai vaksi sebelumnya.</t>
   </si>
 </sst>
 </file>
@@ -417,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -533,6 +551,120 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color indexed="8"/>
       </left>
@@ -542,36 +674,19 @@
       <top style="hair">
         <color indexed="8"/>
       </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color indexed="8"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,32 +695,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -653,54 +748,98 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="24" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="25" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="25" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1150,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1161,129 +1300,63 @@
     <col min="1" max="1" width="28.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
     <col min="3" max="7" width="15.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="21" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="19" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="B2" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="D2" s="30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="F2" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0243055555555556" bottom="1.0243055555555556" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1297,96 +1370,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EEF742-D5FF-4457-91D9-B9A96A506E01}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="31.140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="10"/>
+    <col min="1" max="1" width="7.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="28" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="E2" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="C7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="C8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="E11" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="E13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="E14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="10">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="B19" s="33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="C19" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>